<commit_message>
regional calculations works. cleaning in progress
</commit_message>
<xml_diff>
--- a/config_data/02-Example_spatial_index/spatial_index_example.xlsx
+++ b/config_data/02-Example_spatial_index/spatial_index_example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="22995" windowHeight="11310"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="18255" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>A</t>
   </si>
@@ -96,7 +96,22 @@
     <t>TEST</t>
   </si>
   <si>
-    <t>SUM</t>
+    <t>GWh total in area</t>
+  </si>
+  <si>
+    <t>Service Tech A</t>
+  </si>
+  <si>
+    <t>Service Tech B</t>
+  </si>
+  <si>
+    <t>TEST Tech A</t>
+  </si>
+  <si>
+    <t>Test Tech B</t>
+  </si>
+  <si>
+    <t>Diffusion value (input)</t>
   </si>
 </sst>
 </file>
@@ -112,7 +127,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,8 +152,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -146,16 +173,108 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,10 +576,339 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:P34"/>
+  <dimension ref="C2:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="1.85546875" customWidth="1"/>
+    <col min="13" max="13" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="2">
+        <f>G8*J4</f>
+        <v>1200</v>
+      </c>
+      <c r="N5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D6" s="10"/>
+      <c r="E6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="8">
+        <f>E8/G8</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F7" s="8">
+        <f>F8/G8</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D8" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="8">
+        <f>E10*E9</f>
+        <v>1000</v>
+      </c>
+      <c r="F8" s="8">
+        <f>F10*F9</f>
+        <v>2000</v>
+      </c>
+      <c r="G8" s="14">
+        <f>E8+F8</f>
+        <v>3000</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="2">
+        <f>G8*J7</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D9" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1000</v>
+      </c>
+      <c r="F9" s="8">
+        <v>2000</v>
+      </c>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D10" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D11" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D12" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14">
+        <f>(E11*O4+E12*O5)</f>
+        <v>1.6</v>
+      </c>
+      <c r="F14">
+        <f>(F11*O4+F12*O5)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <f>(E11*O4+E12*O5)/((E11*O4+E12*O5)+(F11*O4+F12*O5))</f>
+        <v>0.39024390243902446</v>
+      </c>
+      <c r="F15">
+        <f xml:space="preserve"> (F11*O4+F12*O5)/((E11*O4+E12*O5) + (F11*O4+F12*O5))</f>
+        <v>0.60975609756097571</v>
+      </c>
+      <c r="G15">
+        <f>E15+F15</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="J15">
+        <f>E14/F14</f>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7">
+        <f>(E14*E7)/((E14*E7+F14*F7))</f>
+        <v>0.24242424242424246</v>
+      </c>
+      <c r="F17" s="7">
+        <f>(F14*F7) / (E7*E14+F7*F14)</f>
+        <v>0.75757575757575757</v>
+      </c>
+      <c r="G17">
+        <f>SUM(F17+E17)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="3"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20">
+        <f>J5*E17</f>
+        <v>290.90909090909093</v>
+      </c>
+      <c r="F20">
+        <f>J5*F17</f>
+        <v>909.09090909090912</v>
+      </c>
+      <c r="G20" s="2">
+        <f>E20+F20</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21">
+        <f>J8*E17</f>
+        <v>436.36363636363643</v>
+      </c>
+      <c r="F21">
+        <f>J8*F17</f>
+        <v>1363.6363636363635</v>
+      </c>
+      <c r="G21" s="2">
+        <f>E21+F21</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f>E21+E20</f>
+        <v>727.27272727272737</v>
+      </c>
+      <c r="F22">
+        <f>F21+F20</f>
+        <v>2272.7272727272725</v>
+      </c>
+      <c r="G22">
+        <f>E22+F22</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24">
+        <f>E20/E8</f>
+        <v>0.29090909090909095</v>
+      </c>
+      <c r="F24">
+        <f>F20/F8</f>
+        <v>0.45454545454545459</v>
+      </c>
+      <c r="G24">
+        <f>SUM(E24:F24)</f>
+        <v>0.74545454545454559</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25">
+        <f>E21/E8</f>
+        <v>0.43636363636363645</v>
+      </c>
+      <c r="F25">
+        <f>F21/F8</f>
+        <v>0.68181818181818177</v>
+      </c>
+      <c r="G25">
+        <f>SUM(E25:F25)</f>
+        <v>1.1181818181818182</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="2">
+        <f>E24*E8+F24*F8</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" s="2">
+        <f>E25*E8+F25*F8</f>
+        <v>1800</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:P36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +943,7 @@
       <c r="I4" s="1">
         <v>0.4</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="5"/>
       <c r="O4" t="s">
         <v>7</v>
       </c>
@@ -520,13 +968,13 @@
       </c>
     </row>
     <row r="6" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -653,7 +1101,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>15</v>
       </c>
@@ -665,139 +1113,183 @@
         <f>(F14*F7) / (E7*E14+F7*F14)</f>
         <v>0.75757575757575757</v>
       </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <f>SUM(F17+E17)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" s="3"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20">
+        <f>E26/E8</f>
+        <v>0.29090909090909095</v>
+      </c>
+      <c r="F20">
+        <f>F26/F8</f>
+        <v>0.45454545454545459</v>
+      </c>
+      <c r="G20">
+        <f>SUM(E20:F20)</f>
+        <v>0.74545454545454559</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21">
+        <f>E27/E8</f>
+        <v>0.43636363636363645</v>
+      </c>
+      <c r="F21">
+        <f>F27/F8</f>
+        <v>0.68181818181818177</v>
+      </c>
+      <c r="G21">
+        <f>SUM(E21:F21)</f>
+        <v>1.1181818181818182</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="2">
+        <f>E20*E8+F20*F8</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24">
+        <f>E17*G8</f>
+        <v>727.27272727272737</v>
+      </c>
+      <c r="F24">
+        <f>F17*G8</f>
+        <v>2272.7272727272725</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>22</v>
       </c>
-      <c r="E24">
+      <c r="E26">
         <f>I5*E17</f>
         <v>290.90909090909093</v>
       </c>
-      <c r="F24">
+      <c r="F26">
         <f>I5*F17</f>
         <v>909.09090909090912</v>
       </c>
-      <c r="G24" s="2">
-        <f>E24+F24</f>
+      <c r="G26" s="2">
+        <f>E26+F26</f>
         <v>1200</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>23</v>
       </c>
-      <c r="E25">
+      <c r="E27">
         <f>I8*E17</f>
         <v>436.36363636363643</v>
       </c>
-      <c r="F25">
+      <c r="F27">
         <f>I8*F17</f>
         <v>1363.6363636363635</v>
       </c>
-      <c r="G25" s="2">
-        <f>E25+F25</f>
+      <c r="G27" s="2">
+        <f>E27+F27</f>
         <v>1800</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26">
-        <f>E25+E24</f>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <f>E27+E26</f>
         <v>727.27272727272737</v>
       </c>
-      <c r="F26">
-        <f>F25+F24</f>
+      <c r="F28">
+        <f>F27+F26</f>
         <v>2272.7272727272725</v>
       </c>
-      <c r="G26">
-        <f>E26+F26</f>
+      <c r="G28">
+        <f>E28+F28</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
         <v>18</v>
       </c>
-      <c r="E28">
-        <f>E24/(E24+E25)</f>
+      <c r="E30">
+        <f>E26/(E26+E27)</f>
         <v>0.39999999999999997</v>
       </c>
-      <c r="F28">
-        <f>F24/(F24+F25)</f>
+      <c r="F30">
+        <f>F26/(F26+F27)</f>
         <v>0.40000000000000008</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>21</v>
       </c>
-      <c r="E29">
-        <f>E25/(E25+E24)</f>
+      <c r="E31">
+        <f>E27/(E27+E26)</f>
         <v>0.6</v>
       </c>
-      <c r="F29">
-        <f>F25/(F25+F24)</f>
+      <c r="F31">
+        <f>F27/(F27+F26)</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E31">
-        <f>E24/G26</f>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <f>E26/G28</f>
         <v>9.6969696969696983E-2</v>
       </c>
-      <c r="F31">
-        <f>F24/G26</f>
+      <c r="F33">
+        <f>F26/G28</f>
         <v>0.30303030303030304</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="E32">
-        <f>E25/G26</f>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <f>E27/G28</f>
         <v>0.14545454545454548</v>
       </c>
-      <c r="F32">
-        <f>F25/G26</f>
+      <c r="F34">
+        <f>F27/G28</f>
         <v>0.45454545454545453</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="4">
-        <f>E28+E29</f>
+      <c r="E35" s="4">
+        <f>E30+E31</f>
         <v>1</v>
       </c>
-      <c r="F33" s="4">
-        <f>F28+F29</f>
+      <c r="F35" s="4">
+        <f>F30+F31</f>
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>